<commit_message>
alterações modelo logico e normalização
</commit_message>
<xml_diff>
--- a/normalização de dados.xlsx
+++ b/normalização de dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio-pc\Documents\facudade\tcc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio -TI\Documents\faculdade\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6BCE3D-A6ED-4374-8F89-8E82589786E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1159E5AA-A510-4CA7-AA1B-97D1CBDAA540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{82851AB4-57C7-4768-AD19-0F0102215559}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{82851AB4-57C7-4768-AD19-0F0102215559}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{C9A3BD3F-E915-4E6B-B994-52208BAAF34D}">
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{C9A3BD3F-E915-4E6B-B994-52208BAAF34D}">
       <text>
         <r>
           <rPr>
@@ -88,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{0B48475E-6356-4BF3-A06D-D7FC9DE555EE}">
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{0B48475E-6356-4BF3-A06D-D7FC9DE555EE}">
       <text>
         <r>
           <rPr>
@@ -114,12 +114,62 @@
         </r>
       </text>
     </comment>
+    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{70422FC8-D4F4-49A4-B53C-0F97F78FEF15}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>fabio -TI:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+normalizar:
+nome
+telefone</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C63" authorId="0" shapeId="0" xr:uid="{367D0889-EBBC-44C0-82A0-E0F6232938FE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>fabio -TI:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+em campo ou em uso</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="171">
   <si>
     <t>Normalização de Dados</t>
   </si>
@@ -223,9 +273,6 @@
     <t>nome_dep</t>
   </si>
   <si>
-    <t>matricula_encarregado</t>
-  </si>
-  <si>
     <t>000001</t>
   </si>
   <si>
@@ -238,9 +285,6 @@
     <t>manutenção</t>
   </si>
   <si>
-    <t>elétrica</t>
-  </si>
-  <si>
     <t>000010</t>
   </si>
   <si>
@@ -313,9 +357,6 @@
     <t xml:space="preserve">mecanico </t>
   </si>
   <si>
-    <t>eletricista</t>
-  </si>
-  <si>
     <t>00030</t>
   </si>
   <si>
@@ -343,12 +384,6 @@
     <t>000042</t>
   </si>
   <si>
-    <t>ligação de quadro elétrico</t>
-  </si>
-  <si>
-    <t>o Funcionário necessita ligar novo quadro eletrico</t>
-  </si>
-  <si>
     <t>fábrica de latas</t>
   </si>
   <si>
@@ -361,50 +396,299 @@
     <t>00051</t>
   </si>
   <si>
-    <t>00052</t>
-  </si>
-  <si>
-    <t>executante1</t>
-  </si>
-  <si>
-    <t>executante2</t>
-  </si>
-  <si>
-    <t>executante3</t>
-  </si>
-  <si>
-    <t>executante4</t>
-  </si>
-  <si>
-    <t>executante5</t>
-  </si>
-  <si>
-    <t>fulano 1</t>
-  </si>
-  <si>
-    <t>fulano 2</t>
-  </si>
-  <si>
-    <t>fulano 3</t>
-  </si>
-  <si>
     <t>executante-tarefa</t>
   </si>
   <si>
     <t>codigo_executante</t>
   </si>
   <si>
-    <t>00053</t>
-  </si>
-  <si>
     <t>00012</t>
+  </si>
+  <si>
+    <t>Manutenção</t>
+  </si>
+  <si>
+    <t>encarregado</t>
+  </si>
+  <si>
+    <t>colaborador</t>
+  </si>
+  <si>
+    <t>000013</t>
+  </si>
+  <si>
+    <t>000004</t>
+  </si>
+  <si>
+    <t>Limpeza</t>
+  </si>
+  <si>
+    <t>000033</t>
+  </si>
+  <si>
+    <t>Serviçõs Gerais</t>
+  </si>
+  <si>
+    <t>ererf</t>
+  </si>
+  <si>
+    <t>Henrrique</t>
+  </si>
+  <si>
+    <t>Fagundes</t>
+  </si>
+  <si>
+    <t>....</t>
+  </si>
+  <si>
+    <t>laboratório</t>
+  </si>
+  <si>
+    <t>Quimica</t>
+  </si>
+  <si>
+    <t>Manipulação de produto quimico</t>
+  </si>
+  <si>
+    <t>o Funcionário necessita manipular produto quimico para analisar a qualidade do produto da fábrica</t>
+  </si>
+  <si>
+    <t>Ficha de E.P.I</t>
+  </si>
+  <si>
+    <t>codigo_ficha_epi</t>
+  </si>
+  <si>
+    <t>codigo_motivo</t>
+  </si>
+  <si>
+    <t>cod_ficha_epi</t>
+  </si>
+  <si>
+    <t>quant_epi</t>
+  </si>
+  <si>
+    <t>nome_epi</t>
+  </si>
+  <si>
+    <t>data_dev_epi</t>
+  </si>
+  <si>
+    <t>obs_entrega</t>
+  </si>
+  <si>
+    <t>data_entrega_epi</t>
+  </si>
+  <si>
+    <t>obs_devolucao</t>
+  </si>
+  <si>
+    <t>tipo_funcionario</t>
+  </si>
+  <si>
+    <t>Encarregado</t>
+  </si>
+  <si>
+    <t>laboratorio</t>
+  </si>
+  <si>
+    <t>limpeza</t>
+  </si>
+  <si>
+    <t>00061</t>
+  </si>
+  <si>
+    <t>Motivo_devolucao</t>
+  </si>
+  <si>
+    <t>00071</t>
+  </si>
+  <si>
+    <t>00072</t>
+  </si>
+  <si>
+    <t>00073</t>
+  </si>
+  <si>
+    <t>00062</t>
+  </si>
+  <si>
+    <t>00063</t>
+  </si>
+  <si>
+    <t>Calça anti-chamas</t>
+  </si>
+  <si>
+    <t>é usado pelo setor de eletrica</t>
+  </si>
+  <si>
+    <t>o epi encontra-se em estado de novo</t>
+  </si>
+  <si>
+    <t>Demissão</t>
+  </si>
+  <si>
+    <t>Adimissção</t>
+  </si>
+  <si>
+    <t>perda</t>
+  </si>
+  <si>
+    <t>roubo</t>
+  </si>
+  <si>
+    <t>extravio</t>
+  </si>
+  <si>
+    <t>vencimento C.A</t>
+  </si>
+  <si>
+    <t>Desgaste Natural</t>
+  </si>
+  <si>
+    <t>00074</t>
+  </si>
+  <si>
+    <t>00075</t>
+  </si>
+  <si>
+    <t>00076</t>
+  </si>
+  <si>
+    <t>00077</t>
+  </si>
+  <si>
+    <t>cod_motivo</t>
+  </si>
+  <si>
+    <t>Nome motivo</t>
+  </si>
+  <si>
+    <t>funcionario-ficha_epi</t>
+  </si>
+  <si>
+    <t>00064</t>
+  </si>
+  <si>
+    <t>Elétrica</t>
+  </si>
+  <si>
+    <t>000014</t>
+  </si>
+  <si>
+    <t>000005</t>
+  </si>
+  <si>
+    <t>Eletricista</t>
+  </si>
+  <si>
+    <t>rerer</t>
+  </si>
+  <si>
+    <t>000034</t>
+  </si>
+  <si>
+    <t>Vinicius</t>
+  </si>
+  <si>
+    <t>Paixao</t>
+  </si>
+  <si>
+    <t>Bairro</t>
+  </si>
+  <si>
+    <t>Huulha Negra</t>
+  </si>
+  <si>
+    <t>capacete</t>
+  </si>
+  <si>
+    <t>o E.P.I foi perdido pelo colaborador, será descontado</t>
+  </si>
+  <si>
+    <t>OBS: estudar o caso do atributo c.a</t>
+  </si>
+  <si>
+    <t>E.P.I</t>
+  </si>
+  <si>
+    <t>cod_epi</t>
+  </si>
+  <si>
+    <t>situação</t>
+  </si>
+  <si>
+    <t>venc.C.A</t>
+  </si>
+  <si>
+    <t>estoque_minimo</t>
+  </si>
+  <si>
+    <t>unidade</t>
+  </si>
+  <si>
+    <t>c.a</t>
+  </si>
+  <si>
+    <t>desc_epi</t>
+  </si>
+  <si>
+    <t>fornecedor</t>
+  </si>
+  <si>
+    <t>data_fabricacao</t>
+  </si>
+  <si>
+    <t>fabricante</t>
+  </si>
+  <si>
+    <t>00081</t>
+  </si>
+  <si>
+    <t>00082</t>
+  </si>
+  <si>
+    <t>00083</t>
+  </si>
+  <si>
+    <t>00084</t>
+  </si>
+  <si>
+    <t>Luva de raspa</t>
+  </si>
+  <si>
+    <t>estoque</t>
+  </si>
+  <si>
+    <t>par</t>
+  </si>
+  <si>
+    <t>luva de uso para armador</t>
+  </si>
+  <si>
+    <t>carbografite</t>
+  </si>
+  <si>
+    <t>fijwara</t>
+  </si>
+  <si>
+    <t>ficha_epi-epi</t>
+  </si>
+  <si>
+    <t>Calça antichamas</t>
+  </si>
+  <si>
+    <t>em campo</t>
+  </si>
+  <si>
+    <t>usado pelo setor de eletrica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,8 +732,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,8 +766,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -529,11 +833,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -551,15 +875,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,6 +882,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -578,21 +907,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -909,10 +1276,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33215026-C023-41C6-931A-1B3971A4E820}">
-  <dimension ref="A1:RP27"/>
+  <dimension ref="A1:RP67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +1288,10 @@
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="24.28515625" customWidth="1"/>
+    <col min="4" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="22" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -928,77 +1299,80 @@
     <col min="14" max="15" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:484" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
     </row>
     <row r="2" spans="1:484" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
     </row>
     <row r="3" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>58</v>
+      <c r="C3" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>23</v>
@@ -1051,8 +1425,12 @@
       <c r="T3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
+      <c r="U3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
@@ -1518,13 +1896,13 @@
     </row>
     <row r="4" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>24</v>
@@ -1577,8 +1955,12 @@
       <c r="T4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
+      <c r="U4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
@@ -2044,19 +2426,19 @@
     </row>
     <row r="5" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F5" s="3">
         <v>4343554</v>
@@ -2103,8 +2485,12 @@
       <c r="T5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
+      <c r="U5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
@@ -2570,19 +2956,19 @@
     </row>
     <row r="6" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" s="3">
         <v>45545</v>
@@ -2597,7 +2983,7 @@
         <v>15</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K6" s="3">
         <v>34354</v>
@@ -2609,7 +2995,7 @@
         <v>23</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O6" s="3">
         <v>53898989</v>
@@ -2627,10 +3013,14 @@
         <v>19</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
@@ -3095,10 +3485,72 @@
       <c r="RP6" s="4"/>
     </row>
     <row r="7" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
+      <c r="A7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="3">
+        <v>54454</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="3">
+        <v>456</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="3">
+        <v>34567</v>
+      </c>
+      <c r="L7" s="3">
+        <v>2312321</v>
+      </c>
+      <c r="M7" s="3">
+        <v>26</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="3">
+        <v>4234234</v>
+      </c>
+      <c r="P7" s="3">
+        <v>4324234</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="3">
+        <v>3234444</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
@@ -3563,28 +4015,72 @@
       <c r="RP7" s="4"/>
     </row>
     <row r="8" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
+      <c r="A8" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" s="3">
+        <v>434355</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="3">
+        <v>459</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K8" s="3">
+        <v>897890</v>
+      </c>
+      <c r="L8" s="3">
+        <v>7987988</v>
+      </c>
+      <c r="M8" s="3">
+        <v>43</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="3">
+        <v>5345345</v>
+      </c>
+      <c r="P8" s="3">
+        <v>5345345</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8" s="27">
+        <v>40992</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
@@ -4049,23 +4545,20 @@
       <c r="RP8" s="4"/>
     </row>
     <row r="9" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9"/>
-      <c r="L9" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
@@ -4538,27 +5031,20 @@
       <c r="RP9" s="4"/>
     </row>
     <row r="10" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -5031,24 +5517,24 @@
       <c r="RP10" s="4"/>
     </row>
     <row r="11" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="A11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11"/>
+      <c r="D11" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
@@ -5521,24 +6007,30 @@
       <c r="RP11" s="4"/>
     </row>
     <row r="12" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="A12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
@@ -6010,253 +6502,1688 @@
       <c r="RO12" s="4"/>
       <c r="RP12" s="4"/>
     </row>
-    <row r="13" spans="1:484" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+      <c r="AG13" s="4"/>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AJ13" s="4"/>
+      <c r="AK13" s="4"/>
+      <c r="AL13" s="4"/>
+      <c r="AM13" s="4"/>
+      <c r="AN13" s="4"/>
+      <c r="AO13" s="4"/>
+      <c r="AP13" s="4"/>
+      <c r="AQ13" s="4"/>
+      <c r="AR13" s="4"/>
+      <c r="AS13" s="4"/>
+      <c r="AT13" s="4"/>
+      <c r="AU13" s="4"/>
+      <c r="AV13" s="4"/>
+      <c r="AW13" s="4"/>
+      <c r="AX13" s="4"/>
+      <c r="AY13" s="4"/>
+      <c r="AZ13" s="4"/>
+      <c r="BA13" s="4"/>
+      <c r="BB13" s="4"/>
+      <c r="BC13" s="4"/>
+      <c r="BD13" s="4"/>
+      <c r="BE13" s="4"/>
+      <c r="BF13" s="4"/>
+      <c r="BG13" s="4"/>
+      <c r="BH13" s="4"/>
+      <c r="BI13" s="4"/>
+      <c r="BJ13" s="4"/>
+      <c r="BK13" s="4"/>
+      <c r="BL13" s="4"/>
+      <c r="BM13" s="4"/>
+      <c r="BN13" s="4"/>
+      <c r="BO13" s="4"/>
+      <c r="BP13" s="4"/>
+      <c r="BQ13" s="4"/>
+      <c r="BR13" s="4"/>
+      <c r="BS13" s="4"/>
+      <c r="BT13" s="4"/>
+      <c r="BU13" s="4"/>
+      <c r="BV13" s="4"/>
+      <c r="BW13" s="4"/>
+      <c r="BX13" s="4"/>
+      <c r="BY13" s="4"/>
+      <c r="BZ13" s="4"/>
+      <c r="CA13" s="4"/>
+      <c r="CB13" s="4"/>
+      <c r="CC13" s="4"/>
+      <c r="CD13" s="4"/>
+      <c r="CE13" s="4"/>
+      <c r="CF13" s="4"/>
+      <c r="CG13" s="4"/>
+      <c r="CH13" s="4"/>
+      <c r="CI13" s="4"/>
+      <c r="CJ13" s="4"/>
+      <c r="CK13" s="4"/>
+      <c r="CL13" s="4"/>
+      <c r="CM13" s="4"/>
+      <c r="CN13" s="4"/>
+      <c r="CO13" s="4"/>
+      <c r="CP13" s="4"/>
+      <c r="CQ13" s="4"/>
+      <c r="CR13" s="4"/>
+      <c r="CS13" s="4"/>
+      <c r="CT13" s="4"/>
+      <c r="CU13" s="4"/>
+      <c r="CV13" s="4"/>
+      <c r="CW13" s="4"/>
+      <c r="CX13" s="4"/>
+      <c r="CY13" s="4"/>
+      <c r="CZ13" s="4"/>
+      <c r="DA13" s="4"/>
+      <c r="DB13" s="4"/>
+      <c r="DC13" s="4"/>
+      <c r="DD13" s="4"/>
+      <c r="DE13" s="4"/>
+      <c r="DF13" s="4"/>
+      <c r="DG13" s="4"/>
+      <c r="DH13" s="4"/>
+      <c r="DI13" s="4"/>
+      <c r="DJ13" s="4"/>
+      <c r="DK13" s="4"/>
+      <c r="DL13" s="4"/>
+      <c r="DM13" s="4"/>
+      <c r="DN13" s="4"/>
+      <c r="DO13" s="4"/>
+      <c r="DP13" s="4"/>
+      <c r="DQ13" s="4"/>
+      <c r="DR13" s="4"/>
+      <c r="DS13" s="4"/>
+      <c r="DT13" s="4"/>
+      <c r="DU13" s="4"/>
+      <c r="DV13" s="4"/>
+      <c r="DW13" s="4"/>
+      <c r="DX13" s="4"/>
+      <c r="DY13" s="4"/>
+      <c r="DZ13" s="4"/>
+      <c r="EA13" s="4"/>
+      <c r="EB13" s="4"/>
+      <c r="EC13" s="4"/>
+      <c r="ED13" s="4"/>
+      <c r="EE13" s="4"/>
+      <c r="EF13" s="4"/>
+      <c r="EG13" s="4"/>
+      <c r="EH13" s="4"/>
+      <c r="EI13" s="4"/>
+      <c r="EJ13" s="4"/>
+      <c r="EK13" s="4"/>
+      <c r="EL13" s="4"/>
+      <c r="EM13" s="4"/>
+      <c r="EN13" s="4"/>
+      <c r="EO13" s="4"/>
+      <c r="EP13" s="4"/>
+      <c r="EQ13" s="4"/>
+      <c r="ER13" s="4"/>
+      <c r="ES13" s="4"/>
+      <c r="ET13" s="4"/>
+      <c r="EU13" s="4"/>
+      <c r="EV13" s="4"/>
+      <c r="EW13" s="4"/>
+      <c r="EX13" s="4"/>
+      <c r="EY13" s="4"/>
+      <c r="EZ13" s="4"/>
+      <c r="FA13" s="4"/>
+      <c r="FB13" s="4"/>
+      <c r="FC13" s="4"/>
+      <c r="FD13" s="4"/>
+      <c r="FE13" s="4"/>
+      <c r="FF13" s="4"/>
+      <c r="FG13" s="4"/>
+      <c r="FH13" s="4"/>
+      <c r="FI13" s="4"/>
+      <c r="FJ13" s="4"/>
+      <c r="FK13" s="4"/>
+      <c r="FL13" s="4"/>
+      <c r="FM13" s="4"/>
+      <c r="FN13" s="4"/>
+      <c r="FO13" s="4"/>
+      <c r="FP13" s="4"/>
+      <c r="FQ13" s="4"/>
+      <c r="FR13" s="4"/>
+      <c r="FS13" s="4"/>
+      <c r="FT13" s="4"/>
+      <c r="FU13" s="4"/>
+      <c r="FV13" s="4"/>
+      <c r="FW13" s="4"/>
+      <c r="FX13" s="4"/>
+      <c r="FY13" s="4"/>
+      <c r="FZ13" s="4"/>
+      <c r="GA13" s="4"/>
+      <c r="GB13" s="4"/>
+      <c r="GC13" s="4"/>
+      <c r="GD13" s="4"/>
+      <c r="GE13" s="4"/>
+      <c r="GF13" s="4"/>
+      <c r="GG13" s="4"/>
+      <c r="GH13" s="4"/>
+      <c r="GI13" s="4"/>
+      <c r="GJ13" s="4"/>
+      <c r="GK13" s="4"/>
+      <c r="GL13" s="4"/>
+      <c r="GM13" s="4"/>
+      <c r="GN13" s="4"/>
+      <c r="GO13" s="4"/>
+      <c r="GP13" s="4"/>
+      <c r="GQ13" s="4"/>
+      <c r="GR13" s="4"/>
+      <c r="GS13" s="4"/>
+      <c r="GT13" s="4"/>
+      <c r="GU13" s="4"/>
+      <c r="GV13" s="4"/>
+      <c r="GW13" s="4"/>
+      <c r="GX13" s="4"/>
+      <c r="GY13" s="4"/>
+      <c r="GZ13" s="4"/>
+      <c r="HA13" s="4"/>
+      <c r="HB13" s="4"/>
+      <c r="HC13" s="4"/>
+      <c r="HD13" s="4"/>
+      <c r="HE13" s="4"/>
+      <c r="HF13" s="4"/>
+      <c r="HG13" s="4"/>
+      <c r="HH13" s="4"/>
+      <c r="HI13" s="4"/>
+      <c r="HJ13" s="4"/>
+      <c r="HK13" s="4"/>
+      <c r="HL13" s="4"/>
+      <c r="HM13" s="4"/>
+      <c r="HN13" s="4"/>
+      <c r="HO13" s="4"/>
+      <c r="HP13" s="4"/>
+      <c r="HQ13" s="4"/>
+      <c r="HR13" s="4"/>
+      <c r="HS13" s="4"/>
+      <c r="HT13" s="4"/>
+      <c r="HU13" s="4"/>
+      <c r="HV13" s="4"/>
+      <c r="HW13" s="4"/>
+      <c r="HX13" s="4"/>
+      <c r="HY13" s="4"/>
+      <c r="HZ13" s="4"/>
+      <c r="IA13" s="4"/>
+      <c r="IB13" s="4"/>
+      <c r="IC13" s="4"/>
+      <c r="ID13" s="4"/>
+      <c r="IE13" s="4"/>
+      <c r="IF13" s="4"/>
+      <c r="IG13" s="4"/>
+      <c r="IH13" s="4"/>
+      <c r="II13" s="4"/>
+      <c r="IJ13" s="4"/>
+      <c r="IK13" s="4"/>
+      <c r="IL13" s="4"/>
+      <c r="IM13" s="4"/>
+      <c r="IN13" s="4"/>
+      <c r="IO13" s="4"/>
+      <c r="IP13" s="4"/>
+      <c r="IQ13" s="4"/>
+      <c r="IR13" s="4"/>
+      <c r="IS13" s="4"/>
+      <c r="IT13" s="4"/>
+      <c r="IU13" s="4"/>
+      <c r="IV13" s="4"/>
+      <c r="IW13" s="4"/>
+      <c r="IX13" s="4"/>
+      <c r="IY13" s="4"/>
+      <c r="IZ13" s="4"/>
+      <c r="JA13" s="4"/>
+      <c r="JB13" s="4"/>
+      <c r="JC13" s="4"/>
+      <c r="JD13" s="4"/>
+      <c r="JE13" s="4"/>
+      <c r="JF13" s="4"/>
+      <c r="JG13" s="4"/>
+      <c r="JH13" s="4"/>
+      <c r="JI13" s="4"/>
+      <c r="JJ13" s="4"/>
+      <c r="JK13" s="4"/>
+      <c r="JL13" s="4"/>
+      <c r="JM13" s="4"/>
+      <c r="JN13" s="4"/>
+      <c r="JO13" s="4"/>
+      <c r="JP13" s="4"/>
+      <c r="JQ13" s="4"/>
+      <c r="JR13" s="4"/>
+      <c r="JS13" s="4"/>
+      <c r="JT13" s="4"/>
+      <c r="JU13" s="4"/>
+      <c r="JV13" s="4"/>
+      <c r="JW13" s="4"/>
+      <c r="JX13" s="4"/>
+      <c r="JY13" s="4"/>
+      <c r="JZ13" s="4"/>
+      <c r="KA13" s="4"/>
+      <c r="KB13" s="4"/>
+      <c r="KC13" s="4"/>
+      <c r="KD13" s="4"/>
+      <c r="KE13" s="4"/>
+      <c r="KF13" s="4"/>
+      <c r="KG13" s="4"/>
+      <c r="KH13" s="4"/>
+      <c r="KI13" s="4"/>
+      <c r="KJ13" s="4"/>
+      <c r="KK13" s="4"/>
+      <c r="KL13" s="4"/>
+      <c r="KM13" s="4"/>
+      <c r="KN13" s="4"/>
+      <c r="KO13" s="4"/>
+      <c r="KP13" s="4"/>
+      <c r="KQ13" s="4"/>
+      <c r="KR13" s="4"/>
+      <c r="KS13" s="4"/>
+      <c r="KT13" s="4"/>
+      <c r="KU13" s="4"/>
+      <c r="KV13" s="4"/>
+      <c r="KW13" s="4"/>
+      <c r="KX13" s="4"/>
+      <c r="KY13" s="4"/>
+      <c r="KZ13" s="4"/>
+      <c r="LA13" s="4"/>
+      <c r="LB13" s="4"/>
+      <c r="LC13" s="4"/>
+      <c r="LD13" s="4"/>
+      <c r="LE13" s="4"/>
+      <c r="LF13" s="4"/>
+      <c r="LG13" s="4"/>
+      <c r="LH13" s="4"/>
+      <c r="LI13" s="4"/>
+      <c r="LJ13" s="4"/>
+      <c r="LK13" s="4"/>
+      <c r="LL13" s="4"/>
+      <c r="LM13" s="4"/>
+      <c r="LN13" s="4"/>
+      <c r="LO13" s="4"/>
+      <c r="LP13" s="4"/>
+      <c r="LQ13" s="4"/>
+      <c r="LR13" s="4"/>
+      <c r="LS13" s="4"/>
+      <c r="LT13" s="4"/>
+      <c r="LU13" s="4"/>
+      <c r="LV13" s="4"/>
+      <c r="LW13" s="4"/>
+      <c r="LX13" s="4"/>
+      <c r="LY13" s="4"/>
+      <c r="LZ13" s="4"/>
+      <c r="MA13" s="4"/>
+      <c r="MB13" s="4"/>
+      <c r="MC13" s="4"/>
+      <c r="MD13" s="4"/>
+      <c r="ME13" s="4"/>
+      <c r="MF13" s="4"/>
+      <c r="MG13" s="4"/>
+      <c r="MH13" s="4"/>
+      <c r="MI13" s="4"/>
+      <c r="MJ13" s="4"/>
+      <c r="MK13" s="4"/>
+      <c r="ML13" s="4"/>
+      <c r="MM13" s="4"/>
+      <c r="MN13" s="4"/>
+      <c r="MO13" s="4"/>
+      <c r="MP13" s="4"/>
+      <c r="MQ13" s="4"/>
+      <c r="MR13" s="4"/>
+      <c r="MS13" s="4"/>
+      <c r="MT13" s="4"/>
+      <c r="MU13" s="4"/>
+      <c r="MV13" s="4"/>
+      <c r="MW13" s="4"/>
+      <c r="MX13" s="4"/>
+      <c r="MY13" s="4"/>
+      <c r="MZ13" s="4"/>
+      <c r="NA13" s="4"/>
+      <c r="NB13" s="4"/>
+      <c r="NC13" s="4"/>
+      <c r="ND13" s="4"/>
+      <c r="NE13" s="4"/>
+      <c r="NF13" s="4"/>
+      <c r="NG13" s="4"/>
+      <c r="NH13" s="4"/>
+      <c r="NI13" s="4"/>
+      <c r="NJ13" s="4"/>
+      <c r="NK13" s="4"/>
+      <c r="NL13" s="4"/>
+      <c r="NM13" s="4"/>
+      <c r="NN13" s="4"/>
+      <c r="NO13" s="4"/>
+      <c r="NP13" s="4"/>
+      <c r="NQ13" s="4"/>
+      <c r="NR13" s="4"/>
+      <c r="NS13" s="4"/>
+      <c r="NT13" s="4"/>
+      <c r="NU13" s="4"/>
+      <c r="NV13" s="4"/>
+      <c r="NW13" s="4"/>
+      <c r="NX13" s="4"/>
+      <c r="NY13" s="4"/>
+      <c r="NZ13" s="4"/>
+      <c r="OA13" s="4"/>
+      <c r="OB13" s="4"/>
+      <c r="OC13" s="4"/>
+      <c r="OD13" s="4"/>
+      <c r="OE13" s="4"/>
+      <c r="OF13" s="4"/>
+      <c r="OG13" s="4"/>
+      <c r="OH13" s="4"/>
+      <c r="OI13" s="4"/>
+      <c r="OJ13" s="4"/>
+      <c r="OK13" s="4"/>
+      <c r="OL13" s="4"/>
+      <c r="OM13" s="4"/>
+      <c r="ON13" s="4"/>
+      <c r="OO13" s="4"/>
+      <c r="OP13" s="4"/>
+      <c r="OQ13" s="4"/>
+      <c r="OR13" s="4"/>
+      <c r="OS13" s="4"/>
+      <c r="OT13" s="4"/>
+      <c r="OU13" s="4"/>
+      <c r="OV13" s="4"/>
+      <c r="OW13" s="4"/>
+      <c r="OX13" s="4"/>
+      <c r="OY13" s="4"/>
+      <c r="OZ13" s="4"/>
+      <c r="PA13" s="4"/>
+      <c r="PB13" s="4"/>
+      <c r="PC13" s="4"/>
+      <c r="PD13" s="4"/>
+      <c r="PE13" s="4"/>
+      <c r="PF13" s="4"/>
+      <c r="PG13" s="4"/>
+      <c r="PH13" s="4"/>
+      <c r="PI13" s="4"/>
+      <c r="PJ13" s="4"/>
+      <c r="PK13" s="4"/>
+      <c r="PL13" s="4"/>
+      <c r="PM13" s="4"/>
+      <c r="PN13" s="4"/>
+      <c r="PO13" s="4"/>
+      <c r="PP13" s="4"/>
+      <c r="PQ13" s="4"/>
+      <c r="PR13" s="4"/>
+      <c r="PS13" s="4"/>
+      <c r="PT13" s="4"/>
+      <c r="PU13" s="4"/>
+      <c r="PV13" s="4"/>
+      <c r="PW13" s="4"/>
+      <c r="PX13" s="4"/>
+      <c r="PY13" s="4"/>
+      <c r="PZ13" s="4"/>
+      <c r="QA13" s="4"/>
+      <c r="QB13" s="4"/>
+      <c r="QC13" s="4"/>
+      <c r="QD13" s="4"/>
+      <c r="QE13" s="4"/>
+      <c r="QF13" s="4"/>
+      <c r="QG13" s="4"/>
+      <c r="QH13" s="4"/>
+      <c r="QI13" s="4"/>
+      <c r="QJ13" s="4"/>
+      <c r="QK13" s="4"/>
+      <c r="QL13" s="4"/>
+      <c r="QM13" s="4"/>
+      <c r="QN13" s="4"/>
+      <c r="QO13" s="4"/>
+      <c r="QP13" s="4"/>
+      <c r="QQ13" s="4"/>
+      <c r="QR13" s="4"/>
+      <c r="QS13" s="4"/>
+      <c r="QT13" s="4"/>
+      <c r="QU13" s="4"/>
+      <c r="QV13" s="4"/>
+      <c r="QW13" s="4"/>
+      <c r="QX13" s="4"/>
+      <c r="QY13" s="4"/>
+      <c r="QZ13" s="4"/>
+      <c r="RA13" s="4"/>
+      <c r="RB13" s="4"/>
+      <c r="RC13" s="4"/>
+      <c r="RD13" s="4"/>
+      <c r="RE13" s="4"/>
+      <c r="RF13" s="4"/>
+      <c r="RG13" s="4"/>
+      <c r="RH13" s="4"/>
+      <c r="RI13" s="4"/>
+      <c r="RJ13" s="4"/>
+      <c r="RK13" s="4"/>
+      <c r="RL13" s="4"/>
+      <c r="RM13" s="4"/>
+      <c r="RN13" s="4"/>
+      <c r="RO13" s="4"/>
+      <c r="RP13" s="4"/>
+    </row>
+    <row r="14" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4"/>
+      <c r="AG14" s="4"/>
+      <c r="AH14" s="4"/>
+      <c r="AI14" s="4"/>
+      <c r="AJ14" s="4"/>
+      <c r="AK14" s="4"/>
+      <c r="AL14" s="4"/>
+      <c r="AM14" s="4"/>
+      <c r="AN14" s="4"/>
+      <c r="AO14" s="4"/>
+      <c r="AP14" s="4"/>
+      <c r="AQ14" s="4"/>
+      <c r="AR14" s="4"/>
+      <c r="AS14" s="4"/>
+      <c r="AT14" s="4"/>
+      <c r="AU14" s="4"/>
+      <c r="AV14" s="4"/>
+      <c r="AW14" s="4"/>
+      <c r="AX14" s="4"/>
+      <c r="AY14" s="4"/>
+      <c r="AZ14" s="4"/>
+      <c r="BA14" s="4"/>
+      <c r="BB14" s="4"/>
+      <c r="BC14" s="4"/>
+      <c r="BD14" s="4"/>
+      <c r="BE14" s="4"/>
+      <c r="BF14" s="4"/>
+      <c r="BG14" s="4"/>
+      <c r="BH14" s="4"/>
+      <c r="BI14" s="4"/>
+      <c r="BJ14" s="4"/>
+      <c r="BK14" s="4"/>
+      <c r="BL14" s="4"/>
+      <c r="BM14" s="4"/>
+      <c r="BN14" s="4"/>
+      <c r="BO14" s="4"/>
+      <c r="BP14" s="4"/>
+      <c r="BQ14" s="4"/>
+      <c r="BR14" s="4"/>
+      <c r="BS14" s="4"/>
+      <c r="BT14" s="4"/>
+      <c r="BU14" s="4"/>
+      <c r="BV14" s="4"/>
+      <c r="BW14" s="4"/>
+      <c r="BX14" s="4"/>
+      <c r="BY14" s="4"/>
+      <c r="BZ14" s="4"/>
+      <c r="CA14" s="4"/>
+      <c r="CB14" s="4"/>
+      <c r="CC14" s="4"/>
+      <c r="CD14" s="4"/>
+      <c r="CE14" s="4"/>
+      <c r="CF14" s="4"/>
+      <c r="CG14" s="4"/>
+      <c r="CH14" s="4"/>
+      <c r="CI14" s="4"/>
+      <c r="CJ14" s="4"/>
+      <c r="CK14" s="4"/>
+      <c r="CL14" s="4"/>
+      <c r="CM14" s="4"/>
+      <c r="CN14" s="4"/>
+      <c r="CO14" s="4"/>
+      <c r="CP14" s="4"/>
+      <c r="CQ14" s="4"/>
+      <c r="CR14" s="4"/>
+      <c r="CS14" s="4"/>
+      <c r="CT14" s="4"/>
+      <c r="CU14" s="4"/>
+      <c r="CV14" s="4"/>
+      <c r="CW14" s="4"/>
+      <c r="CX14" s="4"/>
+      <c r="CY14" s="4"/>
+      <c r="CZ14" s="4"/>
+      <c r="DA14" s="4"/>
+      <c r="DB14" s="4"/>
+      <c r="DC14" s="4"/>
+      <c r="DD14" s="4"/>
+      <c r="DE14" s="4"/>
+      <c r="DF14" s="4"/>
+      <c r="DG14" s="4"/>
+      <c r="DH14" s="4"/>
+      <c r="DI14" s="4"/>
+      <c r="DJ14" s="4"/>
+      <c r="DK14" s="4"/>
+      <c r="DL14" s="4"/>
+      <c r="DM14" s="4"/>
+      <c r="DN14" s="4"/>
+      <c r="DO14" s="4"/>
+      <c r="DP14" s="4"/>
+      <c r="DQ14" s="4"/>
+      <c r="DR14" s="4"/>
+      <c r="DS14" s="4"/>
+      <c r="DT14" s="4"/>
+      <c r="DU14" s="4"/>
+      <c r="DV14" s="4"/>
+      <c r="DW14" s="4"/>
+      <c r="DX14" s="4"/>
+      <c r="DY14" s="4"/>
+      <c r="DZ14" s="4"/>
+      <c r="EA14" s="4"/>
+      <c r="EB14" s="4"/>
+      <c r="EC14" s="4"/>
+      <c r="ED14" s="4"/>
+      <c r="EE14" s="4"/>
+      <c r="EF14" s="4"/>
+      <c r="EG14" s="4"/>
+      <c r="EH14" s="4"/>
+      <c r="EI14" s="4"/>
+      <c r="EJ14" s="4"/>
+      <c r="EK14" s="4"/>
+      <c r="EL14" s="4"/>
+      <c r="EM14" s="4"/>
+      <c r="EN14" s="4"/>
+      <c r="EO14" s="4"/>
+      <c r="EP14" s="4"/>
+      <c r="EQ14" s="4"/>
+      <c r="ER14" s="4"/>
+      <c r="ES14" s="4"/>
+      <c r="ET14" s="4"/>
+      <c r="EU14" s="4"/>
+      <c r="EV14" s="4"/>
+      <c r="EW14" s="4"/>
+      <c r="EX14" s="4"/>
+      <c r="EY14" s="4"/>
+      <c r="EZ14" s="4"/>
+      <c r="FA14" s="4"/>
+      <c r="FB14" s="4"/>
+      <c r="FC14" s="4"/>
+      <c r="FD14" s="4"/>
+      <c r="FE14" s="4"/>
+      <c r="FF14" s="4"/>
+      <c r="FG14" s="4"/>
+      <c r="FH14" s="4"/>
+      <c r="FI14" s="4"/>
+      <c r="FJ14" s="4"/>
+      <c r="FK14" s="4"/>
+      <c r="FL14" s="4"/>
+      <c r="FM14" s="4"/>
+      <c r="FN14" s="4"/>
+      <c r="FO14" s="4"/>
+      <c r="FP14" s="4"/>
+      <c r="FQ14" s="4"/>
+      <c r="FR14" s="4"/>
+      <c r="FS14" s="4"/>
+      <c r="FT14" s="4"/>
+      <c r="FU14" s="4"/>
+      <c r="FV14" s="4"/>
+      <c r="FW14" s="4"/>
+      <c r="FX14" s="4"/>
+      <c r="FY14" s="4"/>
+      <c r="FZ14" s="4"/>
+      <c r="GA14" s="4"/>
+      <c r="GB14" s="4"/>
+      <c r="GC14" s="4"/>
+      <c r="GD14" s="4"/>
+      <c r="GE14" s="4"/>
+      <c r="GF14" s="4"/>
+      <c r="GG14" s="4"/>
+      <c r="GH14" s="4"/>
+      <c r="GI14" s="4"/>
+      <c r="GJ14" s="4"/>
+      <c r="GK14" s="4"/>
+      <c r="GL14" s="4"/>
+      <c r="GM14" s="4"/>
+      <c r="GN14" s="4"/>
+      <c r="GO14" s="4"/>
+      <c r="GP14" s="4"/>
+      <c r="GQ14" s="4"/>
+      <c r="GR14" s="4"/>
+      <c r="GS14" s="4"/>
+      <c r="GT14" s="4"/>
+      <c r="GU14" s="4"/>
+      <c r="GV14" s="4"/>
+      <c r="GW14" s="4"/>
+      <c r="GX14" s="4"/>
+      <c r="GY14" s="4"/>
+      <c r="GZ14" s="4"/>
+      <c r="HA14" s="4"/>
+      <c r="HB14" s="4"/>
+      <c r="HC14" s="4"/>
+      <c r="HD14" s="4"/>
+      <c r="HE14" s="4"/>
+      <c r="HF14" s="4"/>
+      <c r="HG14" s="4"/>
+      <c r="HH14" s="4"/>
+      <c r="HI14" s="4"/>
+      <c r="HJ14" s="4"/>
+      <c r="HK14" s="4"/>
+      <c r="HL14" s="4"/>
+      <c r="HM14" s="4"/>
+      <c r="HN14" s="4"/>
+      <c r="HO14" s="4"/>
+      <c r="HP14" s="4"/>
+      <c r="HQ14" s="4"/>
+      <c r="HR14" s="4"/>
+      <c r="HS14" s="4"/>
+      <c r="HT14" s="4"/>
+      <c r="HU14" s="4"/>
+      <c r="HV14" s="4"/>
+      <c r="HW14" s="4"/>
+      <c r="HX14" s="4"/>
+      <c r="HY14" s="4"/>
+      <c r="HZ14" s="4"/>
+      <c r="IA14" s="4"/>
+      <c r="IB14" s="4"/>
+      <c r="IC14" s="4"/>
+      <c r="ID14" s="4"/>
+      <c r="IE14" s="4"/>
+      <c r="IF14" s="4"/>
+      <c r="IG14" s="4"/>
+      <c r="IH14" s="4"/>
+      <c r="II14" s="4"/>
+      <c r="IJ14" s="4"/>
+      <c r="IK14" s="4"/>
+      <c r="IL14" s="4"/>
+      <c r="IM14" s="4"/>
+      <c r="IN14" s="4"/>
+      <c r="IO14" s="4"/>
+      <c r="IP14" s="4"/>
+      <c r="IQ14" s="4"/>
+      <c r="IR14" s="4"/>
+      <c r="IS14" s="4"/>
+      <c r="IT14" s="4"/>
+      <c r="IU14" s="4"/>
+      <c r="IV14" s="4"/>
+      <c r="IW14" s="4"/>
+      <c r="IX14" s="4"/>
+      <c r="IY14" s="4"/>
+      <c r="IZ14" s="4"/>
+      <c r="JA14" s="4"/>
+      <c r="JB14" s="4"/>
+      <c r="JC14" s="4"/>
+      <c r="JD14" s="4"/>
+      <c r="JE14" s="4"/>
+      <c r="JF14" s="4"/>
+      <c r="JG14" s="4"/>
+      <c r="JH14" s="4"/>
+      <c r="JI14" s="4"/>
+      <c r="JJ14" s="4"/>
+      <c r="JK14" s="4"/>
+      <c r="JL14" s="4"/>
+      <c r="JM14" s="4"/>
+      <c r="JN14" s="4"/>
+      <c r="JO14" s="4"/>
+      <c r="JP14" s="4"/>
+      <c r="JQ14" s="4"/>
+      <c r="JR14" s="4"/>
+      <c r="JS14" s="4"/>
+      <c r="JT14" s="4"/>
+      <c r="JU14" s="4"/>
+      <c r="JV14" s="4"/>
+      <c r="JW14" s="4"/>
+      <c r="JX14" s="4"/>
+      <c r="JY14" s="4"/>
+      <c r="JZ14" s="4"/>
+      <c r="KA14" s="4"/>
+      <c r="KB14" s="4"/>
+      <c r="KC14" s="4"/>
+      <c r="KD14" s="4"/>
+      <c r="KE14" s="4"/>
+      <c r="KF14" s="4"/>
+      <c r="KG14" s="4"/>
+      <c r="KH14" s="4"/>
+      <c r="KI14" s="4"/>
+      <c r="KJ14" s="4"/>
+      <c r="KK14" s="4"/>
+      <c r="KL14" s="4"/>
+      <c r="KM14" s="4"/>
+      <c r="KN14" s="4"/>
+      <c r="KO14" s="4"/>
+      <c r="KP14" s="4"/>
+      <c r="KQ14" s="4"/>
+      <c r="KR14" s="4"/>
+      <c r="KS14" s="4"/>
+      <c r="KT14" s="4"/>
+      <c r="KU14" s="4"/>
+      <c r="KV14" s="4"/>
+      <c r="KW14" s="4"/>
+      <c r="KX14" s="4"/>
+      <c r="KY14" s="4"/>
+      <c r="KZ14" s="4"/>
+      <c r="LA14" s="4"/>
+      <c r="LB14" s="4"/>
+      <c r="LC14" s="4"/>
+      <c r="LD14" s="4"/>
+      <c r="LE14" s="4"/>
+      <c r="LF14" s="4"/>
+      <c r="LG14" s="4"/>
+      <c r="LH14" s="4"/>
+      <c r="LI14" s="4"/>
+      <c r="LJ14" s="4"/>
+      <c r="LK14" s="4"/>
+      <c r="LL14" s="4"/>
+      <c r="LM14" s="4"/>
+      <c r="LN14" s="4"/>
+      <c r="LO14" s="4"/>
+      <c r="LP14" s="4"/>
+      <c r="LQ14" s="4"/>
+      <c r="LR14" s="4"/>
+      <c r="LS14" s="4"/>
+      <c r="LT14" s="4"/>
+      <c r="LU14" s="4"/>
+      <c r="LV14" s="4"/>
+      <c r="LW14" s="4"/>
+      <c r="LX14" s="4"/>
+      <c r="LY14" s="4"/>
+      <c r="LZ14" s="4"/>
+      <c r="MA14" s="4"/>
+      <c r="MB14" s="4"/>
+      <c r="MC14" s="4"/>
+      <c r="MD14" s="4"/>
+      <c r="ME14" s="4"/>
+      <c r="MF14" s="4"/>
+      <c r="MG14" s="4"/>
+      <c r="MH14" s="4"/>
+      <c r="MI14" s="4"/>
+      <c r="MJ14" s="4"/>
+      <c r="MK14" s="4"/>
+      <c r="ML14" s="4"/>
+      <c r="MM14" s="4"/>
+      <c r="MN14" s="4"/>
+      <c r="MO14" s="4"/>
+      <c r="MP14" s="4"/>
+      <c r="MQ14" s="4"/>
+      <c r="MR14" s="4"/>
+      <c r="MS14" s="4"/>
+      <c r="MT14" s="4"/>
+      <c r="MU14" s="4"/>
+      <c r="MV14" s="4"/>
+      <c r="MW14" s="4"/>
+      <c r="MX14" s="4"/>
+      <c r="MY14" s="4"/>
+      <c r="MZ14" s="4"/>
+      <c r="NA14" s="4"/>
+      <c r="NB14" s="4"/>
+      <c r="NC14" s="4"/>
+      <c r="ND14" s="4"/>
+      <c r="NE14" s="4"/>
+      <c r="NF14" s="4"/>
+      <c r="NG14" s="4"/>
+      <c r="NH14" s="4"/>
+      <c r="NI14" s="4"/>
+      <c r="NJ14" s="4"/>
+      <c r="NK14" s="4"/>
+      <c r="NL14" s="4"/>
+      <c r="NM14" s="4"/>
+      <c r="NN14" s="4"/>
+      <c r="NO14" s="4"/>
+      <c r="NP14" s="4"/>
+      <c r="NQ14" s="4"/>
+      <c r="NR14" s="4"/>
+      <c r="NS14" s="4"/>
+      <c r="NT14" s="4"/>
+      <c r="NU14" s="4"/>
+      <c r="NV14" s="4"/>
+      <c r="NW14" s="4"/>
+      <c r="NX14" s="4"/>
+      <c r="NY14" s="4"/>
+      <c r="NZ14" s="4"/>
+      <c r="OA14" s="4"/>
+      <c r="OB14" s="4"/>
+      <c r="OC14" s="4"/>
+      <c r="OD14" s="4"/>
+      <c r="OE14" s="4"/>
+      <c r="OF14" s="4"/>
+      <c r="OG14" s="4"/>
+      <c r="OH14" s="4"/>
+      <c r="OI14" s="4"/>
+      <c r="OJ14" s="4"/>
+      <c r="OK14" s="4"/>
+      <c r="OL14" s="4"/>
+      <c r="OM14" s="4"/>
+      <c r="ON14" s="4"/>
+      <c r="OO14" s="4"/>
+      <c r="OP14" s="4"/>
+      <c r="OQ14" s="4"/>
+      <c r="OR14" s="4"/>
+      <c r="OS14" s="4"/>
+      <c r="OT14" s="4"/>
+      <c r="OU14" s="4"/>
+      <c r="OV14" s="4"/>
+      <c r="OW14" s="4"/>
+      <c r="OX14" s="4"/>
+      <c r="OY14" s="4"/>
+      <c r="OZ14" s="4"/>
+      <c r="PA14" s="4"/>
+      <c r="PB14" s="4"/>
+      <c r="PC14" s="4"/>
+      <c r="PD14" s="4"/>
+      <c r="PE14" s="4"/>
+      <c r="PF14" s="4"/>
+      <c r="PG14" s="4"/>
+      <c r="PH14" s="4"/>
+      <c r="PI14" s="4"/>
+      <c r="PJ14" s="4"/>
+      <c r="PK14" s="4"/>
+      <c r="PL14" s="4"/>
+      <c r="PM14" s="4"/>
+      <c r="PN14" s="4"/>
+      <c r="PO14" s="4"/>
+      <c r="PP14" s="4"/>
+      <c r="PQ14" s="4"/>
+      <c r="PR14" s="4"/>
+      <c r="PS14" s="4"/>
+      <c r="PT14" s="4"/>
+      <c r="PU14" s="4"/>
+      <c r="PV14" s="4"/>
+      <c r="PW14" s="4"/>
+      <c r="PX14" s="4"/>
+      <c r="PY14" s="4"/>
+      <c r="PZ14" s="4"/>
+      <c r="QA14" s="4"/>
+      <c r="QB14" s="4"/>
+      <c r="QC14" s="4"/>
+      <c r="QD14" s="4"/>
+      <c r="QE14" s="4"/>
+      <c r="QF14" s="4"/>
+      <c r="QG14" s="4"/>
+      <c r="QH14" s="4"/>
+      <c r="QI14" s="4"/>
+      <c r="QJ14" s="4"/>
+      <c r="QK14" s="4"/>
+      <c r="QL14" s="4"/>
+      <c r="QM14" s="4"/>
+      <c r="QN14" s="4"/>
+      <c r="QO14" s="4"/>
+      <c r="QP14" s="4"/>
+      <c r="QQ14" s="4"/>
+      <c r="QR14" s="4"/>
+      <c r="QS14" s="4"/>
+      <c r="QT14" s="4"/>
+      <c r="QU14" s="4"/>
+      <c r="QV14" s="4"/>
+      <c r="QW14" s="4"/>
+      <c r="QX14" s="4"/>
+      <c r="QY14" s="4"/>
+      <c r="QZ14" s="4"/>
+      <c r="RA14" s="4"/>
+      <c r="RB14" s="4"/>
+      <c r="RC14" s="4"/>
+      <c r="RD14" s="4"/>
+      <c r="RE14" s="4"/>
+      <c r="RF14" s="4"/>
+      <c r="RG14" s="4"/>
+      <c r="RH14" s="4"/>
+      <c r="RI14" s="4"/>
+      <c r="RJ14" s="4"/>
+      <c r="RK14" s="4"/>
+      <c r="RL14" s="4"/>
+      <c r="RM14" s="4"/>
+      <c r="RN14" s="4"/>
+      <c r="RO14" s="4"/>
+      <c r="RP14" s="4"/>
+    </row>
+    <row r="15" spans="1:484" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:484" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="11">
+        <v>44022</v>
+      </c>
+      <c r="H21" s="11">
+        <v>44022</v>
+      </c>
+      <c r="I21" s="12">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="18"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G34" s="27">
+        <v>44025</v>
+      </c>
+      <c r="H34" s="26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="34">
+        <v>1</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="E35" s="35">
+        <v>44025</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="33">
+        <v>43659</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="37"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" s="32"/>
+      <c r="D39" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" s="18"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="D41" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="B42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="5"/>
     </row>
-    <row r="14" spans="1:484" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="5"/>
     </row>
-    <row r="16" spans="1:484" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="5"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>57</v>
-      </c>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="5"/>
     </row>
-    <row r="18" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L18" s="17">
-        <v>44022</v>
-      </c>
-      <c r="M18" s="17">
-        <v>44022</v>
-      </c>
-      <c r="N18" s="18">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="O18" s="18">
-        <v>0.625</v>
-      </c>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="5"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="5"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="19"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="20"/>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>1</v>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>92</v>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="29" t="s">
+        <v>121</v>
+      </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17"/>
+      <c r="K62" s="18"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E63" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D64" s="11">
+        <v>44756</v>
+      </c>
+      <c r="E64" s="1">
+        <v>12345</v>
+      </c>
+      <c r="F64" s="1">
+        <v>10</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J64" s="11">
+        <v>42868</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D65" s="11">
+        <v>44756</v>
+      </c>
+      <c r="E65" s="1">
+        <v>2455</v>
+      </c>
+      <c r="F65" s="1">
+        <v>20</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J65" s="11">
+        <v>41772</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="A16:O16"/>
+  <mergeCells count="13">
+    <mergeCell ref="A62:K62"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A26:C26"/>
     <mergeCell ref="A2:Y2"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:Y1"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
alteração modelo conceitual e lógico
</commit_message>
<xml_diff>
--- a/normalização de dados.xlsx
+++ b/normalização de dados.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio -TI\Documents\faculdade\tcc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manutenção T.I\Documents\faculdade\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1159E5AA-A510-4CA7-AA1B-97D1CBDAA540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{82851AB4-57C7-4768-AD19-0F0102215559}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>fabio -TI</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{26AE789C-FEA3-418B-9C5C-A373FC9ED89A}">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{C9A3BD3F-E915-4E6B-B994-52208BAAF34D}">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{0B48475E-6356-4BF3-A06D-D7FC9DE555EE}">
+    <comment ref="B21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -114,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{70422FC8-D4F4-49A4-B53C-0F97F78FEF15}">
+    <comment ref="A43" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C63" authorId="0" shapeId="0" xr:uid="{367D0889-EBBC-44C0-82A0-E0F6232938FE}">
+    <comment ref="C63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="190">
   <si>
     <t>Normalização de Dados</t>
   </si>
@@ -606,9 +605,6 @@
     <t>o E.P.I foi perdido pelo colaborador, será descontado</t>
   </si>
   <si>
-    <t>OBS: estudar o caso do atributo c.a</t>
-  </si>
-  <si>
     <t>E.P.I</t>
   </si>
   <si>
@@ -682,12 +678,72 @@
   </si>
   <si>
     <t>usado pelo setor de eletrica</t>
+  </si>
+  <si>
+    <t>codigo_fabricante</t>
+  </si>
+  <si>
+    <t>cidade_fabricante</t>
+  </si>
+  <si>
+    <t>uf_fabricante</t>
+  </si>
+  <si>
+    <t>nome_fabricante</t>
+  </si>
+  <si>
+    <t>telefone_fabricante</t>
+  </si>
+  <si>
+    <t>epi-fabricante</t>
+  </si>
+  <si>
+    <t>codigo_epi</t>
+  </si>
+  <si>
+    <t>epi-fornecedor</t>
+  </si>
+  <si>
+    <t>cod-epi</t>
+  </si>
+  <si>
+    <t>cod_fabricante</t>
+  </si>
+  <si>
+    <t>cod_fornecedor</t>
+  </si>
+  <si>
+    <t>nome_fornecedor</t>
+  </si>
+  <si>
+    <t>rua</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>telefone</t>
+  </si>
+  <si>
+    <t>cep</t>
+  </si>
+  <si>
+    <t>cnpj</t>
+  </si>
+  <si>
+    <t>celular</t>
+  </si>
+  <si>
+    <t>razao_social</t>
+  </si>
+  <si>
+    <t>nome_fantasia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -747,7 +803,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -766,14 +822,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -844,15 +894,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -889,13 +930,32 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -910,13 +970,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -928,39 +1000,8 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1275,12 +1316,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33215026-C023-41C6-931A-1B3971A4E820}">
-  <dimension ref="A1:RP67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:RP83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,62 +1348,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:484" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
     </row>
     <row r="2" spans="1:484" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
     </row>
     <row r="3" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -4066,7 +4107,7 @@
       <c r="Q8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R8" s="27">
+      <c r="R8" s="15">
         <v>40992</v>
       </c>
       <c r="S8" s="3" t="s">
@@ -5517,16 +5558,16 @@
       <c r="RP10" s="4"/>
     </row>
     <row r="11" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="32"/>
       <c r="C11"/>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="27"/>
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
@@ -7498,7 +7539,7 @@
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="13" t="s">
         <v>90</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -7521,10 +7562,10 @@
       <c r="D16" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="13" t="s">
         <v>86</v>
       </c>
     </row>
@@ -7532,32 +7573,32 @@
       <c r="A17" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="13" t="s">
         <v>133</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="13" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="25"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="38"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
@@ -7601,7 +7642,7 @@
       <c r="C21" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="14" t="s">
         <v>93</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -7664,11 +7705,11 @@
       <c r="J24" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
@@ -7703,16 +7744,16 @@
       <c r="C30" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="18"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
@@ -7757,10 +7798,10 @@
       <c r="F34" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G34" s="27">
+      <c r="G34" s="15">
         <v>44025</v>
       </c>
-      <c r="H34" s="26" t="s">
+      <c r="H34" s="14" t="s">
         <v>117</v>
       </c>
     </row>
@@ -7768,23 +7809,23 @@
       <c r="A35" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="C35" s="34">
+      <c r="C35" s="20">
         <v>1</v>
       </c>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="E35" s="35">
+      <c r="E35" s="21">
         <v>44025</v>
       </c>
       <c r="F35" s="10"/>
-      <c r="G35" s="33">
+      <c r="G35" s="19">
         <v>43659</v>
       </c>
-      <c r="H35" s="26" t="s">
+      <c r="H35" s="14" t="s">
         <v>144</v>
       </c>
     </row>
@@ -7805,38 +7846,36 @@
         <v>132</v>
       </c>
       <c r="B37" s="5"/>
-      <c r="C37" s="37" t="s">
-        <v>145</v>
-      </c>
-      <c r="D37" s="37"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="D39" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="D39" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="E39" s="27"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -7850,11 +7889,11 @@
         <v>97</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
+        <v>146</v>
+      </c>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -7866,11 +7905,11 @@
         <v>108</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
+        <v>157</v>
+      </c>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -7880,9 +7919,9 @@
       <c r="B42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -7892,9 +7931,9 @@
       <c r="B43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="30"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -7906,9 +7945,9 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -7920,45 +7959,67 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
       <c r="I47" s="5"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B51" s="19"/>
+      <c r="B51" s="28"/>
+      <c r="D51" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="39" t="s">
+      <c r="A52" s="24" t="s">
         <v>129</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>130</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="E52" t="s">
+        <v>173</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -7968,6 +8029,11 @@
       <c r="B53" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
@@ -7976,6 +8042,11 @@
       <c r="B54" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
@@ -7984,12 +8055,17 @@
       <c r="B55" s="1" t="s">
         <v>120</v>
       </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B56" s="29" t="s">
+      <c r="B56" s="17" t="s">
         <v>121</v>
       </c>
     </row>
@@ -7997,7 +8073,7 @@
       <c r="A57" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B57" s="29" t="s">
+      <c r="B57" s="17" t="s">
         <v>122</v>
       </c>
     </row>
@@ -8005,7 +8081,7 @@
       <c r="A58" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="17" t="s">
         <v>123</v>
       </c>
     </row>
@@ -8013,69 +8089,69 @@
       <c r="A59" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B59" s="29" t="s">
+      <c r="B59" s="17" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="17"/>
-      <c r="K62" s="18"/>
+      <c r="A62" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="27"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="38" t="s">
-        <v>147</v>
+      <c r="A63" s="23" t="s">
+        <v>146</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E63" s="28" t="s">
+      <c r="G63" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H63" s="1" t="s">
+      <c r="I63" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I63" s="1" t="s">
+      <c r="J63" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="J63" s="1" t="s">
+      <c r="K63" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="K63" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="D64" s="11">
         <v>44756</v>
@@ -8087,30 +8163,30 @@
         <v>10</v>
       </c>
       <c r="G64" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="I64" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J64" s="11">
         <v>42868</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="D65" s="11">
         <v>44756</v>
@@ -8122,24 +8198,24 @@
         <v>20</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J65" s="11">
         <v>41772</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -8152,9 +8228,9 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -8167,21 +8243,250 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="B69" s="27"/>
+      <c r="D69" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E69" s="27"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="26"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
+      <c r="G74" s="26"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="26"/>
+      <c r="J74" s="26"/>
+      <c r="K74" s="26"/>
+      <c r="L74" s="26"/>
+      <c r="M74" s="26"/>
+      <c r="N74" s="27"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H75" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N75" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A74:N74"/>
+    <mergeCell ref="A2:Y2"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:Y1"/>
+    <mergeCell ref="D51:H51"/>
     <mergeCell ref="A62:K62"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="A32:H32"/>
-    <mergeCell ref="C37:D37"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A2:Y2"/>
-    <mergeCell ref="A19:J19"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:Y1"/>
+    <mergeCell ref="D69:E69"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
add criação do layout
</commit_message>
<xml_diff>
--- a/normalização de dados.xlsx
+++ b/normalização de dados.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manutenção T.I\Documents\faculdade\tcc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{D70C40BA-C105-674B-8B8C-AE5D2443021A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4827F2E0-0A85-2445-983D-A4FE01F49359}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,12 +33,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>fabio -TI</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0">
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -87,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B21" authorId="0" shapeId="0">
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -113,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A43" authorId="0" shapeId="0">
+    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -139,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C63" authorId="0" shapeId="0">
+    <comment ref="C63" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -168,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="208">
   <si>
     <t>Normalização de Dados</t>
   </si>
@@ -738,13 +741,67 @@
   </si>
   <si>
     <t>nome_fantasia</t>
+  </si>
+  <si>
+    <t>00091</t>
+  </si>
+  <si>
+    <t>00092</t>
+  </si>
+  <si>
+    <t>00093</t>
+  </si>
+  <si>
+    <t>ultra master</t>
+  </si>
+  <si>
+    <t>pelotas</t>
+  </si>
+  <si>
+    <t>msa</t>
+  </si>
+  <si>
+    <t>rio grande</t>
+  </si>
+  <si>
+    <t>00101</t>
+  </si>
+  <si>
+    <t>00102</t>
+  </si>
+  <si>
+    <t>00103</t>
+  </si>
+  <si>
+    <t>00104</t>
+  </si>
+  <si>
+    <t>00105</t>
+  </si>
+  <si>
+    <t>limaseg</t>
+  </si>
+  <si>
+    <t>Manaus</t>
+  </si>
+  <si>
+    <t>npj</t>
+  </si>
+  <si>
+    <t>limasrg</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>yuuhu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -803,7 +860,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -819,6 +876,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,7 +961,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -958,16 +1021,28 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -991,18 +1066,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1316,96 +1384,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:RP83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.05859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.05859375" customWidth="1"/>
+    <col min="3" max="3" width="24.34765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.34765625" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="22" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.34765625" customWidth="1"/>
+    <col min="8" max="8" width="26.09765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="22.05859375" customWidth="1"/>
+    <col min="11" max="11" width="21.65625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.65625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="20.71484375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.46875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.02734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.76171875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.87109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.27734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:484" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:484">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
       <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
     </row>
-    <row r="2" spans="1:484" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:484">
+      <c r="A2" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
     </row>
-    <row r="3" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:484" s="3" customFormat="1">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1935,7 +2003,7 @@
       <c r="RO3" s="4"/>
       <c r="RP3" s="4"/>
     </row>
-    <row r="4" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:484" s="3" customFormat="1">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -2465,7 +2533,7 @@
       <c r="RO4" s="4"/>
       <c r="RP4" s="4"/>
     </row>
-    <row r="5" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:484" s="3" customFormat="1">
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
@@ -2995,7 +3063,7 @@
       <c r="RO5" s="4"/>
       <c r="RP5" s="4"/>
     </row>
-    <row r="6" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:484" s="3" customFormat="1">
       <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
@@ -3525,7 +3593,7 @@
       <c r="RO6" s="4"/>
       <c r="RP6" s="4"/>
     </row>
-    <row r="7" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:484" s="3" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>81</v>
       </c>
@@ -4055,7 +4123,7 @@
       <c r="RO7" s="4"/>
       <c r="RP7" s="4"/>
     </row>
-    <row r="8" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:484" s="3" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>134</v>
       </c>
@@ -4585,7 +4653,7 @@
       <c r="RO8" s="4"/>
       <c r="RP8" s="4"/>
     </row>
-    <row r="9" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:484" s="3" customFormat="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -5071,7 +5139,7 @@
       <c r="RO9" s="4"/>
       <c r="RP9" s="4"/>
     </row>
-    <row r="10" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:484" s="3" customFormat="1">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="4"/>
@@ -5557,16 +5625,16 @@
       <c r="RO10" s="4"/>
       <c r="RP10" s="4"/>
     </row>
-    <row r="11" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+    <row r="11" spans="1:484" s="3" customFormat="1">
+      <c r="A11" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="32"/>
+      <c r="B11" s="36"/>
       <c r="C11"/>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="26"/>
+      <c r="E11" s="28"/>
       <c r="F11" s="27"/>
       <c r="G11"/>
       <c r="H11"/>
@@ -6047,7 +6115,7 @@
       <c r="RO11" s="4"/>
       <c r="RP11" s="4"/>
     </row>
-    <row r="12" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:484" s="3" customFormat="1">
       <c r="A12" s="7" t="s">
         <v>31</v>
       </c>
@@ -6543,7 +6611,7 @@
       <c r="RO12" s="4"/>
       <c r="RP12" s="4"/>
     </row>
-    <row r="13" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:484" s="3" customFormat="1">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -7039,7 +7107,7 @@
       <c r="RO13" s="4"/>
       <c r="RP13" s="4"/>
     </row>
-    <row r="14" spans="1:484" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:484" s="3" customFormat="1">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -7535,7 +7603,7 @@
       <c r="RO14" s="4"/>
       <c r="RP14" s="4"/>
     </row>
-    <row r="15" spans="1:484" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:484">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -7552,7 +7620,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:484" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:484">
       <c r="A16" s="2" t="s">
         <v>82</v>
       </c>
@@ -7569,7 +7637,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
         <v>135</v>
       </c>
@@ -7586,21 +7654,21 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="36" t="s">
+    <row r="19" spans="1:10" ht="18.75">
+      <c r="A19" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="38"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="32"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
@@ -7632,7 +7700,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="36" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -7664,7 +7732,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
         <v>69</v>
       </c>
@@ -7678,7 +7746,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
         <v>70</v>
       </c>
@@ -7692,7 +7760,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="2"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -7704,14 +7772,14 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+    <row r="26" spans="1:10">
+      <c r="A26" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="7" t="s">
         <v>76</v>
       </c>
@@ -7722,7 +7790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -7733,29 +7801,29 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+    <row r="32" spans="1:10">
+      <c r="A32" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
       <c r="H32" s="27"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="7" t="s">
         <v>95</v>
       </c>
@@ -7781,7 +7849,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="27.75">
       <c r="A34" s="2" t="s">
         <v>108</v>
       </c>
@@ -7805,7 +7873,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="27.75">
       <c r="A35" s="2" t="s">
         <v>113</v>
       </c>
@@ -7815,7 +7883,7 @@
       <c r="C35" s="20">
         <v>1</v>
       </c>
-      <c r="D35" s="39" t="s">
+      <c r="D35" s="25" t="s">
         <v>143</v>
       </c>
       <c r="E35" s="21">
@@ -7829,7 +7897,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="2" t="s">
         <v>114</v>
       </c>
@@ -7841,7 +7909,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="2" t="s">
         <v>132</v>
       </c>
@@ -7853,7 +7921,7 @@
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="5"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -7864,12 +7932,12 @@
       <c r="H38" s="18"/>
       <c r="I38" s="5"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="s">
+    <row r="39" spans="1:9">
+      <c r="A39" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="D39" s="25" t="s">
+      <c r="B39" s="34"/>
+      <c r="D39" s="26" t="s">
         <v>166</v>
       </c>
       <c r="E39" s="27"/>
@@ -7878,7 +7946,7 @@
       <c r="H39" s="18"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="9" t="s">
         <v>1</v>
       </c>
@@ -7896,7 +7964,7 @@
       <c r="H40" s="18"/>
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
@@ -7912,7 +7980,7 @@
       <c r="H41" s="18"/>
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
@@ -7924,7 +7992,7 @@
       <c r="H42" s="18"/>
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="2" t="s">
         <v>40</v>
       </c>
@@ -7936,7 +8004,7 @@
       <c r="H43" s="18"/>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" s="2" t="s">
         <v>81</v>
       </c>
@@ -7950,7 +8018,7 @@
       <c r="H44" s="18"/>
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" s="2" t="s">
         <v>134</v>
       </c>
@@ -7964,7 +8032,7 @@
       <c r="H45" s="18"/>
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="5"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -7975,7 +8043,7 @@
       <c r="H46" s="18"/>
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="5"/>
       <c r="B47" s="18"/>
       <c r="C47" s="18"/>
@@ -7986,20 +8054,20 @@
       <c r="H47" s="18"/>
       <c r="I47" s="5"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
+    <row r="51" spans="1:11">
+      <c r="A51" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B51" s="28"/>
-      <c r="D51" s="25" t="s">
+      <c r="B51" s="29"/>
+      <c r="D51" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="A52" s="24" t="s">
         <v>129</v>
       </c>
@@ -8022,46 +8090,68 @@
         <v>174</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="A53" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
+      <c r="D53" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" s="1">
+        <v>53999567842</v>
+      </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11">
       <c r="A54" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="D54" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="1">
+        <v>53999890345</v>
+      </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11">
       <c r="A55" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D55" s="1"/>
+      <c r="D55" s="40" t="s">
+        <v>192</v>
+      </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11">
       <c r="A56" s="2" t="s">
         <v>125</v>
       </c>
@@ -8069,7 +8159,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11">
       <c r="A57" s="2" t="s">
         <v>126</v>
       </c>
@@ -8077,7 +8167,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11">
       <c r="A58" s="2" t="s">
         <v>127</v>
       </c>
@@ -8085,7 +8175,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11">
       <c r="A59" s="2" t="s">
         <v>128</v>
       </c>
@@ -8093,22 +8183,22 @@
         <v>124</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="25" t="s">
+    <row r="62" spans="1:11">
+      <c r="A62" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="26"/>
-      <c r="I62" s="26"/>
-      <c r="J62" s="26"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="28"/>
       <c r="K62" s="27"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11">
       <c r="A63" s="23" t="s">
         <v>146</v>
       </c>
@@ -8143,7 +8233,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11">
       <c r="A64" s="2" t="s">
         <v>156</v>
       </c>
@@ -8178,7 +8268,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14">
       <c r="A65" s="2" t="s">
         <v>157</v>
       </c>
@@ -8213,7 +8303,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14">
       <c r="A66" s="2" t="s">
         <v>158</v>
       </c>
@@ -8228,7 +8318,7 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14">
       <c r="A67" s="2" t="s">
         <v>159</v>
       </c>
@@ -8243,61 +8333,91 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="25" t="s">
+    <row r="69" spans="1:14">
+      <c r="A69" s="26" t="s">
         <v>177</v>
       </c>
       <c r="B69" s="27"/>
-      <c r="D69" s="25" t="s">
+      <c r="D69" s="26" t="s">
         <v>175</v>
       </c>
       <c r="E69" s="27"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="23" t="s">
+    <row r="70" spans="1:14">
+      <c r="A70" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="D70" s="23" t="s">
+      <c r="D70" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" s="42" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
+    <row r="71" spans="1:14">
+      <c r="A71" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>190</v>
+      </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
+    <row r="72" spans="1:14">
+      <c r="A72" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>191</v>
+      </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" s="25" t="s">
+    <row r="73" spans="1:14">
+      <c r="A73" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E73" s="40" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="B74" s="26"/>
-      <c r="C74" s="26"/>
-      <c r="D74" s="26"/>
-      <c r="E74" s="26"/>
-      <c r="F74" s="26"/>
-      <c r="G74" s="26"/>
-      <c r="H74" s="26"/>
-      <c r="I74" s="26"/>
-      <c r="J74" s="26"/>
-      <c r="K74" s="26"/>
-      <c r="L74" s="26"/>
-      <c r="M74" s="26"/>
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="28"/>
+      <c r="G74" s="28"/>
+      <c r="H74" s="28"/>
+      <c r="I74" s="28"/>
+      <c r="J74" s="28"/>
+      <c r="K74" s="28"/>
+      <c r="L74" s="28"/>
+      <c r="M74" s="28"/>
       <c r="N74" s="27"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14">
       <c r="A75" s="23" t="s">
         <v>180</v>
       </c>
@@ -8341,24 +8461,54 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
-      <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
+    <row r="76" spans="1:14">
+      <c r="A76" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E76" s="1">
+        <v>25</v>
+      </c>
+      <c r="F76" s="1">
+        <v>32</v>
+      </c>
+      <c r="G76" s="1">
+        <v>54897654</v>
+      </c>
+      <c r="H76" s="1">
+        <v>54878903</v>
+      </c>
+      <c r="I76" s="1">
+        <v>96325789</v>
+      </c>
+      <c r="J76" s="1">
+        <v>765678999</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>207</v>
+      </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
+    <row r="77" spans="1:14">
+      <c r="A77" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -8373,8 +8523,10 @@
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
+    <row r="78" spans="1:14">
+      <c r="A78" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -8389,8 +8541,10 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
+    <row r="79" spans="1:14">
+      <c r="A79" s="2" t="s">
+        <v>200</v>
+      </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -8405,8 +8559,10 @@
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
+    <row r="80" spans="1:14">
+      <c r="A80" s="2" t="s">
+        <v>201</v>
+      </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -8421,8 +8577,8 @@
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
+    <row r="81" spans="1:14">
+      <c r="A81" s="2"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -8437,7 +8593,7 @@
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -8453,7 +8609,7 @@
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>

</xml_diff>